<commit_message>
test batch for WTP l1 conditions with contrasts
</commit_message>
<xml_diff>
--- a/fMRI/fx/models/WTP/fx_conditions_allwaves_contrast_design.xlsx
+++ b/fMRI/fx/models/WTP/fx_conditions_allwaves_contrast_design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminsmith/Google Drive/oregon/code/DEV_scripts/fMRI/fx/models/WTP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF3E78E-4154-6441-B502-E8A616098BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE3A034-168C-E94D-A41E-67AD743460B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{C2E55B3A-6737-DF4B-B7A9-D1BA84A8D149}"/>
+    <workbookView xWindow="-7860" yWindow="-27940" windowWidth="45020" windowHeight="27160" xr2:uid="{C2E55B3A-6737-DF4B-B7A9-D1BA84A8D149}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -896,16 +896,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45594D6-B9A0-AB4B-9E7E-3ADE9C2DEBB4}">
   <dimension ref="A1:O81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H47" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="185" zoomScaleNormal="185" workbookViewId="0">
+      <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O74" sqref="H74:O81"/>
+      <selection pane="bottomRight" activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="48" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="48" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1054,28 +1054,28 @@
         <v>0</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" ref="I4:I67" si="0">I3&amp;" "&amp;H4</f>
+        <f t="shared" ref="I4:I37" si="0">I3&amp;" "&amp;H4</f>
         <v>-0.25 0 0</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4" t="str">
-        <f t="shared" ref="K4:K67" si="1">K3&amp;" "&amp;J4</f>
+        <f t="shared" ref="K4:K37" si="1">K3&amp;" "&amp;J4</f>
         <v>0 -0.25 0</v>
       </c>
       <c r="L4">
         <v>-0.25</v>
       </c>
       <c r="M4" t="str">
-        <f t="shared" ref="M4:M67" si="2">M3&amp;" "&amp;L4</f>
+        <f t="shared" ref="M4:M37" si="2">M3&amp;" "&amp;L4</f>
         <v>0 0 -0.25</v>
       </c>
       <c r="N4">
         <v>0</v>
       </c>
       <c r="O4" t="str">
-        <f t="shared" ref="O4:O67" si="3">O3&amp;" "&amp;N4</f>
+        <f t="shared" ref="O4:O37" si="3">O3&amp;" "&amp;N4</f>
         <v>0 0 0</v>
       </c>
     </row>
@@ -2788,28 +2788,28 @@
         <v>0.25</v>
       </c>
       <c r="I38" t="str">
-        <f t="shared" ref="I38:I77" si="4">I37&amp;" "&amp;H38</f>
+        <f t="shared" ref="I38:I75" si="4">I37&amp;" "&amp;H38</f>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25</v>
       </c>
       <c r="J38">
         <v>0</v>
       </c>
       <c r="K38" t="str">
-        <f t="shared" ref="K38:K77" si="5">K37&amp;" "&amp;J38</f>
+        <f t="shared" ref="K38:K75" si="5">K37&amp;" "&amp;J38</f>
         <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="L38">
         <v>0</v>
       </c>
       <c r="M38" t="str">
-        <f t="shared" ref="M38:M77" si="6">M37&amp;" "&amp;L38</f>
+        <f t="shared" ref="M38:M75" si="6">M37&amp;" "&amp;L38</f>
         <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0</v>
       </c>
       <c r="N38">
         <v>0</v>
       </c>
       <c r="O38" t="str">
-        <f t="shared" ref="O38:O77" si="7">O37&amp;" "&amp;N38</f>
+        <f t="shared" ref="O38:O75" si="7">O37&amp;" "&amp;N38</f>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
created first level analysis with healthy and unhealthy contrasts
</commit_message>
<xml_diff>
--- a/fMRI/fx/models/WTP/fx_conditions_allwaves_contrast_design.xlsx
+++ b/fMRI/fx/models/WTP/fx_conditions_allwaves_contrast_design.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminsmith/Google Drive/oregon/code/DEV_scripts/fMRI/fx/models/WTP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denicia/DEV/DEV_scripts/fMRI/fx/models/WTP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE3A034-168C-E94D-A41E-67AD743460B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3162D7-3CA2-9B47-9EA4-82F91600966A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7860" yWindow="-27940" windowWidth="45020" windowHeight="27160" xr2:uid="{C2E55B3A-6737-DF4B-B7A9-D1BA84A8D149}"/>
+    <workbookView xWindow="880" yWindow="500" windowWidth="44960" windowHeight="21980" xr2:uid="{C2E55B3A-6737-DF4B-B7A9-D1BA84A8D149}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="173">
   <si>
     <t>'beta_0001.nii'</t>
   </si>
@@ -543,6 +543,18 @@
   </si>
   <si>
     <t>'beta_0080.nii'</t>
+  </si>
+  <si>
+    <t>HealthyVsUnhealthy</t>
+  </si>
+  <si>
+    <t>UnhealthyVsHealthy</t>
+  </si>
+  <si>
+    <t>HealthyLikedVsUnhealthyLiked</t>
+  </si>
+  <si>
+    <t>UnhealthyLikedVsHealthyLiked</t>
   </si>
 </sst>
 </file>
@@ -595,6 +607,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -894,22 +910,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45594D6-B9A0-AB4B-9E7E-3ADE9C2DEBB4}">
-  <dimension ref="A1:O81"/>
+  <dimension ref="A1:W81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="185" zoomScaleNormal="185" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="7" ySplit="1" topLeftCell="H62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A50" sqref="A50"/>
+      <selection pane="bottomRight" activeCell="I96" sqref="I96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="48" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" customWidth="1"/>
+    <col min="9" max="9" width="41.5" customWidth="1"/>
+    <col min="14" max="14" width="25.33203125" customWidth="1"/>
+    <col min="15" max="15" width="2.83203125" customWidth="1"/>
+    <col min="16" max="16" width="35.6640625" customWidth="1"/>
+    <col min="17" max="17" width="222.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.83203125" customWidth="1"/>
+    <col min="19" max="19" width="132.6640625" customWidth="1"/>
+    <col min="20" max="20" width="31" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="37" customWidth="1"/>
+    <col min="23" max="23" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>84</v>
       </c>
@@ -925,8 +952,20 @@
       <c r="N1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P1" t="s">
+        <v>169</v>
+      </c>
+      <c r="R1" t="s">
+        <v>170</v>
+      </c>
+      <c r="T1" t="s">
+        <v>171</v>
+      </c>
+      <c r="V1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -976,8 +1015,37 @@
         <f>N2</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P2">
+        <f>1/16</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q2">
+        <f>P2</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="R2">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="S2">
+        <f>R2</f>
+        <v>-6.25E-2</v>
+      </c>
+      <c r="T2">
+        <v>0.125</v>
+      </c>
+      <c r="U2">
+        <f>T2</f>
+        <v>0.125</v>
+      </c>
+      <c r="V2">
+        <v>-0.125</v>
+      </c>
+      <c r="W2">
+        <f>V2</f>
+        <v>-0.125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1027,8 +1095,36 @@
         <f>O2&amp;" "&amp;N3</f>
         <v>0 0</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P3">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="Q3" t="str">
+        <f>Q2&amp;" "&amp;P3</f>
+        <v>0.0625 -0.0625</v>
+      </c>
+      <c r="R3">
+        <v>6.25E-2</v>
+      </c>
+      <c r="S3" t="str">
+        <f>S2&amp; " "&amp;R3</f>
+        <v>-0.0625 0.0625</v>
+      </c>
+      <c r="T3">
+        <v>-0.125</v>
+      </c>
+      <c r="U3" t="str">
+        <f>U2&amp;" "&amp;T3</f>
+        <v>0.125 -0.125</v>
+      </c>
+      <c r="V3">
+        <v>0.125</v>
+      </c>
+      <c r="W3" t="str">
+        <f>W2&amp;" "&amp;V3</f>
+        <v>-0.125 0.125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1078,8 +1174,36 @@
         <f t="shared" ref="O4:O37" si="3">O3&amp;" "&amp;N4</f>
         <v>0 0 0</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P4">
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q4" t="str">
+        <f>Q3&amp;" "&amp;P4</f>
+        <v>0.0625 -0.0625 0.0625</v>
+      </c>
+      <c r="R4">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="S4" t="str">
+        <f t="shared" ref="S4:S67" si="4">S3&amp; " "&amp;R4</f>
+        <v>-0.0625 0.0625 -0.0625</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4" t="str">
+        <f t="shared" ref="U4:U67" si="5">U3&amp;" "&amp;T4</f>
+        <v>0.125 -0.125 0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4" t="str">
+        <f t="shared" ref="W4:W67" si="6">W3&amp;" "&amp;V4</f>
+        <v>-0.125 0.125 0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1129,8 +1253,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P5">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="Q5" t="str">
+        <f t="shared" ref="Q5:Q68" si="7">Q4&amp;" "&amp;P5</f>
+        <v>0.0625 -0.0625 0.0625 -0.0625</v>
+      </c>
+      <c r="R5">
+        <v>6.25E-2</v>
+      </c>
+      <c r="S5" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1177,11 +1329,39 @@
         <v>0</v>
       </c>
       <c r="O6" t="str">
-        <f t="shared" si="3"/>
+        <f>O5&amp;" "&amp;N6</f>
         <v>0 0 0 -0.25 0</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1231,8 +1411,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1282,8 +1490,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1333,8 +1569,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1384,8 +1648,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1435,8 +1727,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P11">
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q11" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625</v>
+      </c>
+      <c r="R11">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="S11" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625</v>
+      </c>
+      <c r="T11">
+        <v>0.125</v>
+      </c>
+      <c r="U11" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125</v>
+      </c>
+      <c r="V11">
+        <v>-0.125</v>
+      </c>
+      <c r="W11" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1486,8 +1806,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P12">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="Q12" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625</v>
+      </c>
+      <c r="R12">
+        <v>6.25E-2</v>
+      </c>
+      <c r="S12" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625</v>
+      </c>
+      <c r="T12">
+        <v>-0.125</v>
+      </c>
+      <c r="U12" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125</v>
+      </c>
+      <c r="V12">
+        <v>0.125</v>
+      </c>
+      <c r="W12" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1537,8 +1885,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P13">
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q13" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625</v>
+      </c>
+      <c r="R13">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="S13" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1588,8 +1964,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P14">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="Q14" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625</v>
+      </c>
+      <c r="R14">
+        <v>6.25E-2</v>
+      </c>
+      <c r="S14" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1639,8 +2043,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1690,8 +2122,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1741,8 +2201,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1792,8 +2280,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1843,8 +2359,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1894,8 +2438,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P20">
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q20" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625</v>
+      </c>
+      <c r="R20">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="S20" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625</v>
+      </c>
+      <c r="T20">
+        <v>0.125</v>
+      </c>
+      <c r="U20" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125</v>
+      </c>
+      <c r="V20">
+        <v>-0.125</v>
+      </c>
+      <c r="W20" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1945,8 +2517,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P21">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="Q21" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625</v>
+      </c>
+      <c r="R21">
+        <v>6.25E-2</v>
+      </c>
+      <c r="S21" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625</v>
+      </c>
+      <c r="T21">
+        <v>-0.125</v>
+      </c>
+      <c r="U21" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125</v>
+      </c>
+      <c r="V21">
+        <v>0.125</v>
+      </c>
+      <c r="W21" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1996,8 +2596,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P22">
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q22" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625</v>
+      </c>
+      <c r="R22">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="S22" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2047,8 +2675,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P23">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="Q23" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625</v>
+      </c>
+      <c r="R23">
+        <v>6.25E-2</v>
+      </c>
+      <c r="S23" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2098,8 +2754,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1</v>
       </c>
@@ -2149,8 +2833,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -2200,8 +2912,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="U26" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
@@ -2251,8 +2991,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -2302,8 +3070,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -2353,8 +3149,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P29">
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q29" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625</v>
+      </c>
+      <c r="R29">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="S29" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625</v>
+      </c>
+      <c r="T29">
+        <v>0.125</v>
+      </c>
+      <c r="U29" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125</v>
+      </c>
+      <c r="V29">
+        <v>-0.125</v>
+      </c>
+      <c r="W29" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
@@ -2404,8 +3228,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P30">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="Q30" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625</v>
+      </c>
+      <c r="R30">
+        <v>6.25E-2</v>
+      </c>
+      <c r="S30" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625</v>
+      </c>
+      <c r="T30">
+        <v>-0.125</v>
+      </c>
+      <c r="U30" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125</v>
+      </c>
+      <c r="V30">
+        <v>0.125</v>
+      </c>
+      <c r="W30" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -2455,8 +3307,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P31">
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q31" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625</v>
+      </c>
+      <c r="R31">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="S31" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625</v>
+      </c>
+      <c r="T31">
+        <v>0</v>
+      </c>
+      <c r="U31" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0</v>
+      </c>
+      <c r="V31">
+        <v>0</v>
+      </c>
+      <c r="W31" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2506,8 +3386,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P32">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="Q32" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625</v>
+      </c>
+      <c r="R32">
+        <v>6.25E-2</v>
+      </c>
+      <c r="S32" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625</v>
+      </c>
+      <c r="T32">
+        <v>0</v>
+      </c>
+      <c r="U32" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0</v>
+      </c>
+      <c r="V32">
+        <v>0</v>
+      </c>
+      <c r="W32" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1</v>
       </c>
@@ -2557,8 +3465,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P33">
+        <v>0</v>
+      </c>
+      <c r="Q33" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0</v>
+      </c>
+      <c r="R33">
+        <v>0</v>
+      </c>
+      <c r="S33" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0</v>
+      </c>
+      <c r="T33">
+        <v>0</v>
+      </c>
+      <c r="U33" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0</v>
+      </c>
+      <c r="V33">
+        <v>0</v>
+      </c>
+      <c r="W33" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1</v>
       </c>
@@ -2608,8 +3544,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="Q34" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0</v>
+      </c>
+      <c r="R34">
+        <v>0</v>
+      </c>
+      <c r="S34" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0</v>
+      </c>
+      <c r="T34">
+        <v>0</v>
+      </c>
+      <c r="U34" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0</v>
+      </c>
+      <c r="V34">
+        <v>0</v>
+      </c>
+      <c r="W34" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1</v>
       </c>
@@ -2659,8 +3623,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0</v>
+      </c>
+      <c r="R35">
+        <v>0</v>
+      </c>
+      <c r="S35" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0</v>
+      </c>
+      <c r="T35">
+        <v>0</v>
+      </c>
+      <c r="U35" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0</v>
+      </c>
+      <c r="V35">
+        <v>0</v>
+      </c>
+      <c r="W35" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1</v>
       </c>
@@ -2710,8 +3702,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="Q36" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0</v>
+      </c>
+      <c r="R36">
+        <v>0</v>
+      </c>
+      <c r="S36" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0</v>
+      </c>
+      <c r="T36">
+        <v>0</v>
+      </c>
+      <c r="U36" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0</v>
+      </c>
+      <c r="V36">
+        <v>0</v>
+      </c>
+      <c r="W36" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
@@ -2761,8 +3781,36 @@
         <f t="shared" si="3"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="Q37" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0</v>
+      </c>
+      <c r="R37">
+        <v>0</v>
+      </c>
+      <c r="S37" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0</v>
+      </c>
+      <c r="T37">
+        <v>0</v>
+      </c>
+      <c r="U37" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="V37">
+        <v>0</v>
+      </c>
+      <c r="W37" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2</v>
       </c>
@@ -2788,32 +3836,60 @@
         <v>0.25</v>
       </c>
       <c r="I38" t="str">
-        <f t="shared" ref="I38:I75" si="4">I37&amp;" "&amp;H38</f>
+        <f t="shared" ref="I38:I75" si="8">I37&amp;" "&amp;H38</f>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25</v>
       </c>
       <c r="J38">
         <v>0</v>
       </c>
       <c r="K38" t="str">
-        <f t="shared" ref="K38:K75" si="5">K37&amp;" "&amp;J38</f>
+        <f t="shared" ref="K38:K75" si="9">K37&amp;" "&amp;J38</f>
         <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="L38">
         <v>0</v>
       </c>
       <c r="M38" t="str">
-        <f t="shared" ref="M38:M75" si="6">M37&amp;" "&amp;L38</f>
+        <f t="shared" ref="M38:M75" si="10">M37&amp;" "&amp;L38</f>
         <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0</v>
       </c>
       <c r="N38">
         <v>0</v>
       </c>
       <c r="O38" t="str">
-        <f t="shared" ref="O38:O75" si="7">O37&amp;" "&amp;N38</f>
+        <f t="shared" ref="O38:O75" si="11">O37&amp;" "&amp;N38</f>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P38">
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q38" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625</v>
+      </c>
+      <c r="R38">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="S38" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625</v>
+      </c>
+      <c r="T38">
+        <v>0.125</v>
+      </c>
+      <c r="U38" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125</v>
+      </c>
+      <c r="V38">
+        <v>-0.125</v>
+      </c>
+      <c r="W38" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2</v>
       </c>
@@ -2839,32 +3915,60 @@
         <v>0</v>
       </c>
       <c r="I39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0</v>
       </c>
       <c r="J39">
         <v>0.25</v>
       </c>
       <c r="K39" t="str">
+        <f t="shared" si="9"/>
+        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="P39">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="Q39" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625</v>
+      </c>
+      <c r="R39">
+        <v>6.25E-2</v>
+      </c>
+      <c r="S39" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625</v>
+      </c>
+      <c r="T39">
+        <v>-0.125</v>
+      </c>
+      <c r="U39" t="str">
         <f t="shared" si="5"/>
-        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25</v>
-      </c>
-      <c r="L39">
-        <v>0</v>
-      </c>
-      <c r="M39" t="str">
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125</v>
+      </c>
+      <c r="V39">
+        <v>0.125</v>
+      </c>
+      <c r="W39" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0</v>
-      </c>
-      <c r="N39">
-        <v>0</v>
-      </c>
-      <c r="O39" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2</v>
       </c>
@@ -2890,32 +3994,60 @@
         <v>0</v>
       </c>
       <c r="I40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0</v>
       </c>
       <c r="J40">
         <v>0</v>
       </c>
       <c r="K40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0</v>
       </c>
       <c r="L40">
         <v>0.25</v>
       </c>
       <c r="M40" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="P40">
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q40" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625</v>
+      </c>
+      <c r="R40">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="S40" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625</v>
+      </c>
+      <c r="T40">
+        <v>0</v>
+      </c>
+      <c r="U40" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0</v>
+      </c>
+      <c r="V40">
+        <v>0</v>
+      </c>
+      <c r="W40" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25</v>
-      </c>
-      <c r="N40">
-        <v>0</v>
-      </c>
-      <c r="O40" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2</v>
       </c>
@@ -2941,32 +4073,60 @@
         <v>0</v>
       </c>
       <c r="I41" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0</v>
       </c>
       <c r="J41">
         <v>0</v>
       </c>
       <c r="K41" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0</v>
       </c>
       <c r="L41">
         <v>0</v>
       </c>
       <c r="M41" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0</v>
       </c>
       <c r="N41">
         <v>0.25</v>
       </c>
       <c r="O41" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25</v>
+      </c>
+      <c r="P41">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="Q41" t="str">
         <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625</v>
+      </c>
+      <c r="R41">
+        <v>6.25E-2</v>
+      </c>
+      <c r="S41" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625</v>
+      </c>
+      <c r="T41">
+        <v>0</v>
+      </c>
+      <c r="U41" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0</v>
+      </c>
+      <c r="V41">
+        <v>0</v>
+      </c>
+      <c r="W41" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2</v>
       </c>
@@ -2992,32 +4152,60 @@
         <v>0</v>
       </c>
       <c r="I42" t="str">
+        <f t="shared" si="8"/>
+        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42" t="str">
+        <f t="shared" si="9"/>
+        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0</v>
+      </c>
+      <c r="P42">
+        <v>0</v>
+      </c>
+      <c r="Q42" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0</v>
+      </c>
+      <c r="R42">
+        <v>0</v>
+      </c>
+      <c r="S42" t="str">
         <f t="shared" si="4"/>
-        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
-      </c>
-      <c r="J42">
-        <v>0</v>
-      </c>
-      <c r="K42" t="str">
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0</v>
+      </c>
+      <c r="T42">
+        <v>0</v>
+      </c>
+      <c r="U42" t="str">
         <f t="shared" si="5"/>
-        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0</v>
-      </c>
-      <c r="L42">
-        <v>0</v>
-      </c>
-      <c r="M42" t="str">
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0</v>
+      </c>
+      <c r="V42">
+        <v>0</v>
+      </c>
+      <c r="W42" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0</v>
-      </c>
-      <c r="N42">
-        <v>0</v>
-      </c>
-      <c r="O42" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2</v>
       </c>
@@ -3043,32 +4231,60 @@
         <v>0</v>
       </c>
       <c r="I43" t="str">
+        <f t="shared" si="8"/>
+        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43" t="str">
+        <f t="shared" si="9"/>
+        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+      <c r="M43" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0</v>
+      </c>
+      <c r="P43">
+        <v>0</v>
+      </c>
+      <c r="Q43" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0</v>
+      </c>
+      <c r="R43">
+        <v>0</v>
+      </c>
+      <c r="S43" t="str">
         <f t="shared" si="4"/>
-        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
-      </c>
-      <c r="J43">
-        <v>0</v>
-      </c>
-      <c r="K43" t="str">
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0</v>
+      </c>
+      <c r="T43">
+        <v>0</v>
+      </c>
+      <c r="U43" t="str">
         <f t="shared" si="5"/>
-        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
-      </c>
-      <c r="L43">
-        <v>0</v>
-      </c>
-      <c r="M43" t="str">
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0</v>
+      </c>
+      <c r="V43">
+        <v>0</v>
+      </c>
+      <c r="W43" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0</v>
-      </c>
-      <c r="N43">
-        <v>0</v>
-      </c>
-      <c r="O43" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2</v>
       </c>
@@ -3094,32 +4310,60 @@
         <v>0</v>
       </c>
       <c r="I44" t="str">
+        <f t="shared" si="8"/>
+        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44" t="str">
+        <f t="shared" si="9"/>
+        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0</v>
+      </c>
+      <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="Q44" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0</v>
+      </c>
+      <c r="R44">
+        <v>0</v>
+      </c>
+      <c r="S44" t="str">
         <f t="shared" si="4"/>
-        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
-      </c>
-      <c r="J44">
-        <v>0</v>
-      </c>
-      <c r="K44" t="str">
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0</v>
+      </c>
+      <c r="T44">
+        <v>0</v>
+      </c>
+      <c r="U44" t="str">
         <f t="shared" si="5"/>
-        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
-      </c>
-      <c r="L44">
-        <v>0</v>
-      </c>
-      <c r="M44" t="str">
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0</v>
+      </c>
+      <c r="V44">
+        <v>0</v>
+      </c>
+      <c r="W44" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
-      </c>
-      <c r="N44">
-        <v>0</v>
-      </c>
-      <c r="O44" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2</v>
       </c>
@@ -3145,32 +4389,60 @@
         <v>0</v>
       </c>
       <c r="I45" t="str">
+        <f t="shared" si="8"/>
+        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45" t="str">
+        <f t="shared" si="9"/>
+        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
+      </c>
+      <c r="P45">
+        <v>0</v>
+      </c>
+      <c r="Q45" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0</v>
+      </c>
+      <c r="R45">
+        <v>0</v>
+      </c>
+      <c r="S45" t="str">
         <f t="shared" si="4"/>
-        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
-      </c>
-      <c r="J45">
-        <v>0</v>
-      </c>
-      <c r="K45" t="str">
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0</v>
+      </c>
+      <c r="T45">
+        <v>0</v>
+      </c>
+      <c r="U45" t="str">
         <f t="shared" si="5"/>
-        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
-      </c>
-      <c r="L45">
-        <v>0</v>
-      </c>
-      <c r="M45" t="str">
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0</v>
+      </c>
+      <c r="V45">
+        <v>0</v>
+      </c>
+      <c r="W45" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
-      </c>
-      <c r="N45">
-        <v>0</v>
-      </c>
-      <c r="O45" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2</v>
       </c>
@@ -3196,32 +4468,60 @@
         <v>0</v>
       </c>
       <c r="I46" t="str">
+        <f t="shared" si="8"/>
+        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46" t="str">
+        <f t="shared" si="9"/>
+        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
+      </c>
+      <c r="P46">
+        <v>0</v>
+      </c>
+      <c r="Q46" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0</v>
+      </c>
+      <c r="R46">
+        <v>0</v>
+      </c>
+      <c r="S46" t="str">
         <f t="shared" si="4"/>
-        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
-      </c>
-      <c r="J46">
-        <v>0</v>
-      </c>
-      <c r="K46" t="str">
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0</v>
+      </c>
+      <c r="T46">
+        <v>0</v>
+      </c>
+      <c r="U46" t="str">
         <f t="shared" si="5"/>
-        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
-      </c>
-      <c r="L46">
-        <v>0</v>
-      </c>
-      <c r="M46" t="str">
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="V46">
+        <v>0</v>
+      </c>
+      <c r="W46" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
-      </c>
-      <c r="N46">
-        <v>0</v>
-      </c>
-      <c r="O46" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2</v>
       </c>
@@ -3247,32 +4547,60 @@
         <v>0.25</v>
       </c>
       <c r="I47" t="str">
+        <f t="shared" si="8"/>
+        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47" t="str">
+        <f t="shared" si="9"/>
+        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
+      </c>
+      <c r="P47">
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q47" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625</v>
+      </c>
+      <c r="R47">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="S47" t="str">
         <f t="shared" si="4"/>
-        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25</v>
-      </c>
-      <c r="J47">
-        <v>0</v>
-      </c>
-      <c r="K47" t="str">
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625</v>
+      </c>
+      <c r="T47">
+        <v>0.125</v>
+      </c>
+      <c r="U47" t="str">
         <f t="shared" si="5"/>
-        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
-      </c>
-      <c r="L47">
-        <v>0</v>
-      </c>
-      <c r="M47" t="str">
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125</v>
+      </c>
+      <c r="V47">
+        <v>-0.125</v>
+      </c>
+      <c r="W47" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
-      </c>
-      <c r="N47">
-        <v>0</v>
-      </c>
-      <c r="O47" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2</v>
       </c>
@@ -3298,32 +4626,60 @@
         <v>0</v>
       </c>
       <c r="I48" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0</v>
       </c>
       <c r="J48">
         <v>0.25</v>
       </c>
       <c r="K48" t="str">
+        <f t="shared" si="9"/>
+        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="O48" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="P48">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="Q48" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625</v>
+      </c>
+      <c r="R48">
+        <v>6.25E-2</v>
+      </c>
+      <c r="S48" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625</v>
+      </c>
+      <c r="T48">
+        <v>-0.125</v>
+      </c>
+      <c r="U48" t="str">
         <f t="shared" si="5"/>
-        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25</v>
-      </c>
-      <c r="L48">
-        <v>0</v>
-      </c>
-      <c r="M48" t="str">
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125</v>
+      </c>
+      <c r="V48">
+        <v>0.125</v>
+      </c>
+      <c r="W48" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
-      </c>
-      <c r="N48">
-        <v>0</v>
-      </c>
-      <c r="O48" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2</v>
       </c>
@@ -3349,32 +4705,60 @@
         <v>0</v>
       </c>
       <c r="I49" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0</v>
       </c>
       <c r="J49">
         <v>0</v>
       </c>
       <c r="K49" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0</v>
       </c>
       <c r="L49">
         <v>0.25</v>
       </c>
       <c r="M49" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
+      <c r="O49" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="P49">
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q49" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625</v>
+      </c>
+      <c r="R49">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="S49" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625</v>
+      </c>
+      <c r="T49">
+        <v>0</v>
+      </c>
+      <c r="U49" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0</v>
+      </c>
+      <c r="V49">
+        <v>0</v>
+      </c>
+      <c r="W49" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25</v>
-      </c>
-      <c r="N49">
-        <v>0</v>
-      </c>
-      <c r="O49" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2</v>
       </c>
@@ -3400,32 +4784,60 @@
         <v>0</v>
       </c>
       <c r="I50" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0</v>
       </c>
       <c r="J50">
         <v>0</v>
       </c>
       <c r="K50" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0</v>
       </c>
       <c r="L50">
         <v>0</v>
       </c>
       <c r="M50" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0</v>
       </c>
       <c r="N50">
         <v>0.25</v>
       </c>
       <c r="O50" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25</v>
+      </c>
+      <c r="P50">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="Q50" t="str">
         <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625</v>
+      </c>
+      <c r="R50">
+        <v>6.25E-2</v>
+      </c>
+      <c r="S50" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625</v>
+      </c>
+      <c r="T50">
+        <v>0</v>
+      </c>
+      <c r="U50" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0</v>
+      </c>
+      <c r="V50">
+        <v>0</v>
+      </c>
+      <c r="W50" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>2</v>
       </c>
@@ -3451,32 +4863,60 @@
         <v>0</v>
       </c>
       <c r="I51" t="str">
+        <f t="shared" si="8"/>
+        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51" t="str">
+        <f t="shared" si="9"/>
+        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+      <c r="M51" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0</v>
+      </c>
+      <c r="N51">
+        <v>0</v>
+      </c>
+      <c r="O51" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0</v>
+      </c>
+      <c r="P51">
+        <v>0</v>
+      </c>
+      <c r="Q51" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0</v>
+      </c>
+      <c r="R51">
+        <v>0</v>
+      </c>
+      <c r="S51" t="str">
         <f t="shared" si="4"/>
-        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
-      </c>
-      <c r="J51">
-        <v>0</v>
-      </c>
-      <c r="K51" t="str">
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0</v>
+      </c>
+      <c r="T51">
+        <v>0</v>
+      </c>
+      <c r="U51" t="str">
         <f t="shared" si="5"/>
-        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0</v>
-      </c>
-      <c r="L51">
-        <v>0</v>
-      </c>
-      <c r="M51" t="str">
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0</v>
+      </c>
+      <c r="V51">
+        <v>0</v>
+      </c>
+      <c r="W51" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0</v>
-      </c>
-      <c r="N51">
-        <v>0</v>
-      </c>
-      <c r="O51" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2</v>
       </c>
@@ -3502,32 +4942,60 @@
         <v>0</v>
       </c>
       <c r="I52" t="str">
+        <f t="shared" si="8"/>
+        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52" t="str">
+        <f t="shared" si="9"/>
+        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+      <c r="M52" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0</v>
+      </c>
+      <c r="N52">
+        <v>0</v>
+      </c>
+      <c r="O52" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0</v>
+      </c>
+      <c r="P52">
+        <v>0</v>
+      </c>
+      <c r="Q52" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0</v>
+      </c>
+      <c r="R52">
+        <v>0</v>
+      </c>
+      <c r="S52" t="str">
         <f t="shared" si="4"/>
-        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
-      </c>
-      <c r="J52">
-        <v>0</v>
-      </c>
-      <c r="K52" t="str">
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0</v>
+      </c>
+      <c r="T52">
+        <v>0</v>
+      </c>
+      <c r="U52" t="str">
         <f t="shared" si="5"/>
-        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
-      </c>
-      <c r="L52">
-        <v>0</v>
-      </c>
-      <c r="M52" t="str">
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0</v>
+      </c>
+      <c r="V52">
+        <v>0</v>
+      </c>
+      <c r="W52" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0</v>
-      </c>
-      <c r="N52">
-        <v>0</v>
-      </c>
-      <c r="O52" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2</v>
       </c>
@@ -3553,32 +5021,60 @@
         <v>0</v>
       </c>
       <c r="I53" t="str">
+        <f t="shared" si="8"/>
+        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53" t="str">
+        <f t="shared" si="9"/>
+        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="M53" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
+      </c>
+      <c r="N53">
+        <v>0</v>
+      </c>
+      <c r="O53" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0</v>
+      </c>
+      <c r="P53">
+        <v>0</v>
+      </c>
+      <c r="Q53" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0</v>
+      </c>
+      <c r="R53">
+        <v>0</v>
+      </c>
+      <c r="S53" t="str">
         <f t="shared" si="4"/>
-        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
-      </c>
-      <c r="J53">
-        <v>0</v>
-      </c>
-      <c r="K53" t="str">
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0</v>
+      </c>
+      <c r="T53">
+        <v>0</v>
+      </c>
+      <c r="U53" t="str">
         <f t="shared" si="5"/>
-        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
-      </c>
-      <c r="L53">
-        <v>0</v>
-      </c>
-      <c r="M53" t="str">
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0</v>
+      </c>
+      <c r="V53">
+        <v>0</v>
+      </c>
+      <c r="W53" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
-      </c>
-      <c r="N53">
-        <v>0</v>
-      </c>
-      <c r="O53" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2</v>
       </c>
@@ -3604,32 +5100,60 @@
         <v>0</v>
       </c>
       <c r="I54" t="str">
+        <f t="shared" si="8"/>
+        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54" t="str">
+        <f t="shared" si="9"/>
+        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+      <c r="M54" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
+      </c>
+      <c r="N54">
+        <v>0</v>
+      </c>
+      <c r="O54" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
+      </c>
+      <c r="P54">
+        <v>0</v>
+      </c>
+      <c r="Q54" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0</v>
+      </c>
+      <c r="R54">
+        <v>0</v>
+      </c>
+      <c r="S54" t="str">
         <f t="shared" si="4"/>
-        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
-      </c>
-      <c r="J54">
-        <v>0</v>
-      </c>
-      <c r="K54" t="str">
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0</v>
+      </c>
+      <c r="T54">
+        <v>0</v>
+      </c>
+      <c r="U54" t="str">
         <f t="shared" si="5"/>
-        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
-      </c>
-      <c r="L54">
-        <v>0</v>
-      </c>
-      <c r="M54" t="str">
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0</v>
+      </c>
+      <c r="V54">
+        <v>0</v>
+      </c>
+      <c r="W54" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
-      </c>
-      <c r="N54">
-        <v>0</v>
-      </c>
-      <c r="O54" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2</v>
       </c>
@@ -3655,32 +5179,60 @@
         <v>0</v>
       </c>
       <c r="I55" t="str">
+        <f t="shared" si="8"/>
+        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55" t="str">
+        <f t="shared" si="9"/>
+        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
+      <c r="M55" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
+      </c>
+      <c r="N55">
+        <v>0</v>
+      </c>
+      <c r="O55" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
+      </c>
+      <c r="P55">
+        <v>0</v>
+      </c>
+      <c r="Q55" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0</v>
+      </c>
+      <c r="R55">
+        <v>0</v>
+      </c>
+      <c r="S55" t="str">
         <f t="shared" si="4"/>
-        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
-      </c>
-      <c r="J55">
-        <v>0</v>
-      </c>
-      <c r="K55" t="str">
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0</v>
+      </c>
+      <c r="T55">
+        <v>0</v>
+      </c>
+      <c r="U55" t="str">
         <f t="shared" si="5"/>
-        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
-      </c>
-      <c r="L55">
-        <v>0</v>
-      </c>
-      <c r="M55" t="str">
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="V55">
+        <v>0</v>
+      </c>
+      <c r="W55" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
-      </c>
-      <c r="N55">
-        <v>0</v>
-      </c>
-      <c r="O55" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>2</v>
       </c>
@@ -3706,32 +5258,60 @@
         <v>0.25</v>
       </c>
       <c r="I56" t="str">
+        <f t="shared" si="8"/>
+        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56" t="str">
+        <f t="shared" si="9"/>
+        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
+      <c r="M56" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="N56">
+        <v>0</v>
+      </c>
+      <c r="O56" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
+      </c>
+      <c r="P56">
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q56" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625</v>
+      </c>
+      <c r="R56">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="S56" t="str">
         <f t="shared" si="4"/>
-        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25</v>
-      </c>
-      <c r="J56">
-        <v>0</v>
-      </c>
-      <c r="K56" t="str">
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625</v>
+      </c>
+      <c r="T56">
+        <v>0.125</v>
+      </c>
+      <c r="U56" t="str">
         <f t="shared" si="5"/>
-        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
-      </c>
-      <c r="L56">
-        <v>0</v>
-      </c>
-      <c r="M56" t="str">
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125</v>
+      </c>
+      <c r="V56">
+        <v>-0.125</v>
+      </c>
+      <c r="W56" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
-      </c>
-      <c r="N56">
-        <v>0</v>
-      </c>
-      <c r="O56" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>2</v>
       </c>
@@ -3757,32 +5337,60 @@
         <v>0</v>
       </c>
       <c r="I57" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0</v>
       </c>
       <c r="J57">
         <v>0.25</v>
       </c>
       <c r="K57" t="str">
+        <f t="shared" si="9"/>
+        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
+      <c r="M57" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="N57">
+        <v>0</v>
+      </c>
+      <c r="O57" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="P57">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="Q57" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625</v>
+      </c>
+      <c r="R57">
+        <v>6.25E-2</v>
+      </c>
+      <c r="S57" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625</v>
+      </c>
+      <c r="T57">
+        <v>-0.125</v>
+      </c>
+      <c r="U57" t="str">
         <f t="shared" si="5"/>
-        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25</v>
-      </c>
-      <c r="L57">
-        <v>0</v>
-      </c>
-      <c r="M57" t="str">
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125</v>
+      </c>
+      <c r="V57">
+        <v>0.125</v>
+      </c>
+      <c r="W57" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
-      </c>
-      <c r="N57">
-        <v>0</v>
-      </c>
-      <c r="O57" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>2</v>
       </c>
@@ -3808,32 +5416,60 @@
         <v>0</v>
       </c>
       <c r="I58" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0</v>
       </c>
       <c r="J58">
         <v>0</v>
       </c>
       <c r="K58" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0</v>
       </c>
       <c r="L58">
         <v>0.25</v>
       </c>
       <c r="M58" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25</v>
+      </c>
+      <c r="N58">
+        <v>0</v>
+      </c>
+      <c r="O58" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="P58">
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q58" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625</v>
+      </c>
+      <c r="R58">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="S58" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625</v>
+      </c>
+      <c r="T58">
+        <v>0</v>
+      </c>
+      <c r="U58" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0</v>
+      </c>
+      <c r="V58">
+        <v>0</v>
+      </c>
+      <c r="W58" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25</v>
-      </c>
-      <c r="N58">
-        <v>0</v>
-      </c>
-      <c r="O58" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2</v>
       </c>
@@ -3859,32 +5495,60 @@
         <v>0</v>
       </c>
       <c r="I59" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0</v>
       </c>
       <c r="J59">
         <v>0</v>
       </c>
       <c r="K59" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0</v>
       </c>
       <c r="L59">
         <v>0</v>
       </c>
       <c r="M59" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0</v>
       </c>
       <c r="N59">
         <v>0.25</v>
       </c>
       <c r="O59" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25</v>
+      </c>
+      <c r="P59">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="Q59" t="str">
         <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625</v>
+      </c>
+      <c r="R59">
+        <v>6.25E-2</v>
+      </c>
+      <c r="S59" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625</v>
+      </c>
+      <c r="T59">
+        <v>0</v>
+      </c>
+      <c r="U59" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0</v>
+      </c>
+      <c r="V59">
+        <v>0</v>
+      </c>
+      <c r="W59" t="str">
+        <f t="shared" si="6"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>2</v>
       </c>
@@ -3910,32 +5574,60 @@
         <v>0</v>
       </c>
       <c r="I60" t="str">
+        <f t="shared" si="8"/>
+        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60" t="str">
+        <f t="shared" si="9"/>
+        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0</v>
+      </c>
+      <c r="L60">
+        <v>0</v>
+      </c>
+      <c r="M60" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0</v>
+      </c>
+      <c r="N60">
+        <v>0</v>
+      </c>
+      <c r="O60" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0</v>
+      </c>
+      <c r="P60">
+        <v>0</v>
+      </c>
+      <c r="Q60" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0</v>
+      </c>
+      <c r="R60">
+        <v>0</v>
+      </c>
+      <c r="S60" t="str">
         <f t="shared" si="4"/>
-        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
-      </c>
-      <c r="J60">
-        <v>0</v>
-      </c>
-      <c r="K60" t="str">
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0</v>
+      </c>
+      <c r="T60">
+        <v>0</v>
+      </c>
+      <c r="U60" t="str">
         <f t="shared" si="5"/>
-        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0</v>
-      </c>
-      <c r="L60">
-        <v>0</v>
-      </c>
-      <c r="M60" t="str">
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0</v>
+      </c>
+      <c r="V60">
+        <v>0</v>
+      </c>
+      <c r="W60" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0</v>
-      </c>
-      <c r="N60">
-        <v>0</v>
-      </c>
-      <c r="O60" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>2</v>
       </c>
@@ -3961,32 +5653,60 @@
         <v>0</v>
       </c>
       <c r="I61" t="str">
+        <f t="shared" si="8"/>
+        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+      <c r="K61" t="str">
+        <f t="shared" si="9"/>
+        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
+      <c r="M61" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0</v>
+      </c>
+      <c r="N61">
+        <v>0</v>
+      </c>
+      <c r="O61" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0</v>
+      </c>
+      <c r="P61">
+        <v>0</v>
+      </c>
+      <c r="Q61" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0</v>
+      </c>
+      <c r="R61">
+        <v>0</v>
+      </c>
+      <c r="S61" t="str">
         <f t="shared" si="4"/>
-        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
-      </c>
-      <c r="J61">
-        <v>0</v>
-      </c>
-      <c r="K61" t="str">
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0</v>
+      </c>
+      <c r="T61">
+        <v>0</v>
+      </c>
+      <c r="U61" t="str">
         <f t="shared" si="5"/>
-        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
-      </c>
-      <c r="L61">
-        <v>0</v>
-      </c>
-      <c r="M61" t="str">
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0</v>
+      </c>
+      <c r="V61">
+        <v>0</v>
+      </c>
+      <c r="W61" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0</v>
-      </c>
-      <c r="N61">
-        <v>0</v>
-      </c>
-      <c r="O61" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2</v>
       </c>
@@ -4012,32 +5732,60 @@
         <v>0</v>
       </c>
       <c r="I62" t="str">
+        <f t="shared" si="8"/>
+        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="K62" t="str">
+        <f t="shared" si="9"/>
+        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
+      </c>
+      <c r="L62">
+        <v>0</v>
+      </c>
+      <c r="M62" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
+      </c>
+      <c r="N62">
+        <v>0</v>
+      </c>
+      <c r="O62" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0</v>
+      </c>
+      <c r="P62">
+        <v>0</v>
+      </c>
+      <c r="Q62" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0</v>
+      </c>
+      <c r="R62">
+        <v>0</v>
+      </c>
+      <c r="S62" t="str">
         <f t="shared" si="4"/>
-        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
-      </c>
-      <c r="J62">
-        <v>0</v>
-      </c>
-      <c r="K62" t="str">
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0</v>
+      </c>
+      <c r="T62">
+        <v>0</v>
+      </c>
+      <c r="U62" t="str">
         <f t="shared" si="5"/>
-        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
-      </c>
-      <c r="L62">
-        <v>0</v>
-      </c>
-      <c r="M62" t="str">
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0</v>
+      </c>
+      <c r="V62">
+        <v>0</v>
+      </c>
+      <c r="W62" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
-      </c>
-      <c r="N62">
-        <v>0</v>
-      </c>
-      <c r="O62" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>2</v>
       </c>
@@ -4063,32 +5811,60 @@
         <v>0</v>
       </c>
       <c r="I63" t="str">
+        <f t="shared" si="8"/>
+        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+      <c r="K63" t="str">
+        <f t="shared" si="9"/>
+        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
+      </c>
+      <c r="L63">
+        <v>0</v>
+      </c>
+      <c r="M63" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
+      </c>
+      <c r="N63">
+        <v>0</v>
+      </c>
+      <c r="O63" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
+      </c>
+      <c r="P63">
+        <v>0</v>
+      </c>
+      <c r="Q63" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0</v>
+      </c>
+      <c r="R63">
+        <v>0</v>
+      </c>
+      <c r="S63" t="str">
         <f t="shared" si="4"/>
-        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
-      </c>
-      <c r="J63">
-        <v>0</v>
-      </c>
-      <c r="K63" t="str">
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0</v>
+      </c>
+      <c r="T63">
+        <v>0</v>
+      </c>
+      <c r="U63" t="str">
         <f t="shared" si="5"/>
-        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
-      </c>
-      <c r="L63">
-        <v>0</v>
-      </c>
-      <c r="M63" t="str">
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0</v>
+      </c>
+      <c r="V63">
+        <v>0</v>
+      </c>
+      <c r="W63" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
-      </c>
-      <c r="N63">
-        <v>0</v>
-      </c>
-      <c r="O63" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>2</v>
       </c>
@@ -4114,32 +5890,60 @@
         <v>0</v>
       </c>
       <c r="I64" t="str">
+        <f t="shared" si="8"/>
+        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="K64" t="str">
+        <f t="shared" si="9"/>
+        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="L64">
+        <v>0</v>
+      </c>
+      <c r="M64" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
+      </c>
+      <c r="N64">
+        <v>0</v>
+      </c>
+      <c r="O64" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
+      </c>
+      <c r="P64">
+        <v>0</v>
+      </c>
+      <c r="Q64" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0</v>
+      </c>
+      <c r="R64">
+        <v>0</v>
+      </c>
+      <c r="S64" t="str">
         <f t="shared" si="4"/>
-        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
-      </c>
-      <c r="J64">
-        <v>0</v>
-      </c>
-      <c r="K64" t="str">
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0</v>
+      </c>
+      <c r="T64">
+        <v>0</v>
+      </c>
+      <c r="U64" t="str">
         <f t="shared" si="5"/>
-        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
-      </c>
-      <c r="L64">
-        <v>0</v>
-      </c>
-      <c r="M64" t="str">
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="V64">
+        <v>0</v>
+      </c>
+      <c r="W64" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
-      </c>
-      <c r="N64">
-        <v>0</v>
-      </c>
-      <c r="O64" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2</v>
       </c>
@@ -4165,32 +5969,60 @@
         <v>0.25</v>
       </c>
       <c r="I65" t="str">
+        <f t="shared" si="8"/>
+        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="K65" t="str">
+        <f t="shared" si="9"/>
+        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="L65">
+        <v>0</v>
+      </c>
+      <c r="M65" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="N65">
+        <v>0</v>
+      </c>
+      <c r="O65" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
+      </c>
+      <c r="P65">
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q65" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625</v>
+      </c>
+      <c r="R65">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="S65" t="str">
         <f t="shared" si="4"/>
-        <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25</v>
-      </c>
-      <c r="J65">
-        <v>0</v>
-      </c>
-      <c r="K65" t="str">
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625</v>
+      </c>
+      <c r="T65">
+        <v>0.125</v>
+      </c>
+      <c r="U65" t="str">
         <f t="shared" si="5"/>
-        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
-      </c>
-      <c r="L65">
-        <v>0</v>
-      </c>
-      <c r="M65" t="str">
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125</v>
+      </c>
+      <c r="V65">
+        <v>-0.125</v>
+      </c>
+      <c r="W65" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
-      </c>
-      <c r="N65">
-        <v>0</v>
-      </c>
-      <c r="O65" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>2</v>
       </c>
@@ -4216,32 +6048,60 @@
         <v>0</v>
       </c>
       <c r="I66" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0</v>
       </c>
       <c r="J66">
         <v>0.25</v>
       </c>
       <c r="K66" t="str">
+        <f t="shared" si="9"/>
+        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25</v>
+      </c>
+      <c r="L66">
+        <v>0</v>
+      </c>
+      <c r="M66" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="N66">
+        <v>0</v>
+      </c>
+      <c r="O66" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="P66">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="Q66" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625</v>
+      </c>
+      <c r="R66">
+        <v>6.25E-2</v>
+      </c>
+      <c r="S66" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625</v>
+      </c>
+      <c r="T66">
+        <v>-0.125</v>
+      </c>
+      <c r="U66" t="str">
         <f t="shared" si="5"/>
-        <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25</v>
-      </c>
-      <c r="L66">
-        <v>0</v>
-      </c>
-      <c r="M66" t="str">
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125</v>
+      </c>
+      <c r="V66">
+        <v>0.125</v>
+      </c>
+      <c r="W66" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
-      </c>
-      <c r="N66">
-        <v>0</v>
-      </c>
-      <c r="O66" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125</v>
+      </c>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2</v>
       </c>
@@ -4267,32 +6127,60 @@
         <v>0</v>
       </c>
       <c r="I67" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0</v>
       </c>
       <c r="J67">
         <v>0</v>
       </c>
       <c r="K67" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0</v>
       </c>
       <c r="L67">
         <v>0.25</v>
       </c>
       <c r="M67" t="str">
+        <f t="shared" si="10"/>
+        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25</v>
+      </c>
+      <c r="N67">
+        <v>0</v>
+      </c>
+      <c r="O67" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="P67">
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q67" t="str">
+        <f t="shared" si="7"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625</v>
+      </c>
+      <c r="R67">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="S67" t="str">
+        <f t="shared" si="4"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625</v>
+      </c>
+      <c r="T67">
+        <v>0</v>
+      </c>
+      <c r="U67" t="str">
+        <f t="shared" si="5"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0</v>
+      </c>
+      <c r="V67">
+        <v>0</v>
+      </c>
+      <c r="W67" t="str">
         <f t="shared" si="6"/>
-        <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25</v>
-      </c>
-      <c r="N67">
-        <v>0</v>
-      </c>
-      <c r="O67" t="str">
-        <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>2</v>
       </c>
@@ -4318,32 +6206,60 @@
         <v>0</v>
       </c>
       <c r="I68" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0</v>
       </c>
       <c r="J68">
         <v>0</v>
       </c>
       <c r="K68" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0</v>
       </c>
       <c r="L68">
         <v>0</v>
       </c>
       <c r="M68" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0</v>
       </c>
       <c r="N68">
         <v>0.25</v>
       </c>
       <c r="O68" t="str">
+        <f t="shared" si="11"/>
+        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25</v>
+      </c>
+      <c r="P68">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="Q68" t="str">
         <f t="shared" si="7"/>
-        <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625</v>
+      </c>
+      <c r="R68">
+        <v>6.25E-2</v>
+      </c>
+      <c r="S68" t="str">
+        <f t="shared" ref="S68:S81" si="12">S67&amp; " "&amp;R68</f>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625</v>
+      </c>
+      <c r="T68">
+        <v>0</v>
+      </c>
+      <c r="U68" t="str">
+        <f t="shared" ref="U68:U81" si="13">U67&amp;" "&amp;T68</f>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0</v>
+      </c>
+      <c r="V68">
+        <v>0</v>
+      </c>
+      <c r="W68" t="str">
+        <f t="shared" ref="W68:W81" si="14">W67&amp;" "&amp;V68</f>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>2</v>
       </c>
@@ -4369,32 +6285,60 @@
         <v>0</v>
       </c>
       <c r="I69" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
       </c>
       <c r="J69">
         <v>0</v>
       </c>
       <c r="K69" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0</v>
       </c>
       <c r="L69">
         <v>0</v>
       </c>
       <c r="M69" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0</v>
       </c>
       <c r="N69">
         <v>0</v>
       </c>
       <c r="O69" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P69">
+        <v>0</v>
+      </c>
+      <c r="Q69" t="str">
+        <f t="shared" ref="Q69:Q81" si="15">Q68&amp;" "&amp;P69</f>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0</v>
+      </c>
+      <c r="R69">
+        <v>0</v>
+      </c>
+      <c r="S69" t="str">
+        <f t="shared" si="12"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0</v>
+      </c>
+      <c r="T69">
+        <v>0</v>
+      </c>
+      <c r="U69" t="str">
+        <f t="shared" si="13"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0</v>
+      </c>
+      <c r="V69">
+        <v>0</v>
+      </c>
+      <c r="W69" t="str">
+        <f t="shared" si="14"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>2</v>
       </c>
@@ -4420,32 +6364,60 @@
         <v>0</v>
       </c>
       <c r="I70" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
       </c>
       <c r="J70">
         <v>0</v>
       </c>
       <c r="K70" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
       </c>
       <c r="L70">
         <v>0</v>
       </c>
       <c r="M70" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0</v>
       </c>
       <c r="N70">
         <v>0</v>
       </c>
       <c r="O70" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P70">
+        <v>0</v>
+      </c>
+      <c r="Q70" t="str">
+        <f t="shared" si="15"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0</v>
+      </c>
+      <c r="R70">
+        <v>0</v>
+      </c>
+      <c r="S70" t="str">
+        <f t="shared" si="12"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0</v>
+      </c>
+      <c r="T70">
+        <v>0</v>
+      </c>
+      <c r="U70" t="str">
+        <f t="shared" si="13"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0</v>
+      </c>
+      <c r="V70">
+        <v>0</v>
+      </c>
+      <c r="W70" t="str">
+        <f t="shared" si="14"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>2</v>
       </c>
@@ -4471,32 +6443,60 @@
         <v>0</v>
       </c>
       <c r="I71" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
       </c>
       <c r="J71">
         <v>0</v>
       </c>
       <c r="K71" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
       </c>
       <c r="L71">
         <v>0</v>
       </c>
       <c r="M71" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
       </c>
       <c r="N71">
         <v>0</v>
       </c>
       <c r="O71" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P71">
+        <v>0</v>
+      </c>
+      <c r="Q71" t="str">
+        <f t="shared" si="15"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0</v>
+      </c>
+      <c r="R71">
+        <v>0</v>
+      </c>
+      <c r="S71" t="str">
+        <f t="shared" si="12"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0</v>
+      </c>
+      <c r="T71">
+        <v>0</v>
+      </c>
+      <c r="U71" t="str">
+        <f t="shared" si="13"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0</v>
+      </c>
+      <c r="V71">
+        <v>0</v>
+      </c>
+      <c r="W71" t="str">
+        <f t="shared" si="14"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>2</v>
       </c>
@@ -4522,32 +6522,60 @@
         <v>0</v>
       </c>
       <c r="I72" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
       </c>
       <c r="J72">
         <v>0</v>
       </c>
       <c r="K72" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
       </c>
       <c r="L72">
         <v>0</v>
       </c>
       <c r="M72" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
       </c>
       <c r="N72">
         <v>0</v>
       </c>
       <c r="O72" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P72">
+        <v>0</v>
+      </c>
+      <c r="Q72" t="str">
+        <f t="shared" si="15"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0</v>
+      </c>
+      <c r="R72">
+        <v>0</v>
+      </c>
+      <c r="S72" t="str">
+        <f t="shared" si="12"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0</v>
+      </c>
+      <c r="T72">
+        <v>0</v>
+      </c>
+      <c r="U72" t="str">
+        <f t="shared" si="13"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0</v>
+      </c>
+      <c r="V72">
+        <v>0</v>
+      </c>
+      <c r="W72" t="str">
+        <f t="shared" si="14"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>2</v>
       </c>
@@ -4573,32 +6601,60 @@
         <v>0</v>
       </c>
       <c r="I73" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="J73">
         <v>0</v>
       </c>
       <c r="K73" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
       </c>
       <c r="L73">
         <v>0</v>
       </c>
       <c r="M73" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
       </c>
       <c r="N73">
         <v>0</v>
       </c>
       <c r="O73" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P73">
+        <v>0</v>
+      </c>
+      <c r="Q73" t="str">
+        <f t="shared" si="15"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0</v>
+      </c>
+      <c r="R73">
+        <v>0</v>
+      </c>
+      <c r="S73" t="str">
+        <f t="shared" si="12"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0</v>
+      </c>
+      <c r="T73">
+        <v>0</v>
+      </c>
+      <c r="U73" t="str">
+        <f t="shared" si="13"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="V73">
+        <v>0</v>
+      </c>
+      <c r="W73" t="str">
+        <f t="shared" si="14"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>1</v>
       </c>
@@ -4624,32 +6680,60 @@
         <v>0</v>
       </c>
       <c r="I74" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="J74">
         <v>0</v>
       </c>
       <c r="K74" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="L74">
         <v>0</v>
       </c>
       <c r="M74" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
       </c>
       <c r="N74">
         <v>0</v>
       </c>
       <c r="O74" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P74">
+        <v>0</v>
+      </c>
+      <c r="Q74" t="str">
+        <f t="shared" si="15"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0</v>
+      </c>
+      <c r="R74">
+        <v>0</v>
+      </c>
+      <c r="S74" t="str">
+        <f t="shared" si="12"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 0</v>
+      </c>
+      <c r="T74">
+        <v>0</v>
+      </c>
+      <c r="U74" t="str">
+        <f t="shared" si="13"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="V74">
+        <v>0</v>
+      </c>
+      <c r="W74" t="str">
+        <f t="shared" si="14"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>1</v>
       </c>
@@ -4675,32 +6759,60 @@
         <v>0</v>
       </c>
       <c r="I75" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="J75">
         <v>0</v>
       </c>
       <c r="K75" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="L75">
         <v>0</v>
       </c>
       <c r="M75" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="N75">
         <v>0</v>
       </c>
       <c r="O75" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P75">
+        <v>0</v>
+      </c>
+      <c r="Q75" t="str">
+        <f t="shared" si="15"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="R75">
+        <v>0</v>
+      </c>
+      <c r="S75" t="str">
+        <f t="shared" si="12"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="T75">
+        <v>0</v>
+      </c>
+      <c r="U75" t="str">
+        <f t="shared" si="13"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="V75">
+        <v>0</v>
+      </c>
+      <c r="W75" t="str">
+        <f t="shared" si="14"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>1</v>
       </c>
@@ -4726,32 +6838,60 @@
         <v>0</v>
       </c>
       <c r="I76" t="str">
-        <f t="shared" ref="I76:I81" si="8">I75&amp;" "&amp;H76</f>
+        <f t="shared" ref="I76:I81" si="16">I75&amp;" "&amp;H76</f>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="J76">
         <v>0</v>
       </c>
       <c r="K76" t="str">
-        <f t="shared" ref="K76:K81" si="9">K75&amp;" "&amp;J76</f>
+        <f t="shared" ref="K76:K81" si="17">K75&amp;" "&amp;J76</f>
         <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="L76">
         <v>0</v>
       </c>
       <c r="M76" t="str">
-        <f t="shared" ref="M76:M81" si="10">M75&amp;" "&amp;L76</f>
+        <f t="shared" ref="M76:M81" si="18">M75&amp;" "&amp;L76</f>
         <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="N76">
         <v>0</v>
       </c>
       <c r="O76" t="str">
-        <f t="shared" ref="O76:O81" si="11">O75&amp;" "&amp;N76</f>
+        <f t="shared" ref="O76:O81" si="19">O75&amp;" "&amp;N76</f>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P76">
+        <v>0</v>
+      </c>
+      <c r="Q76" t="str">
+        <f t="shared" si="15"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="R76">
+        <v>0</v>
+      </c>
+      <c r="S76" t="str">
+        <f t="shared" si="12"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="T76">
+        <v>0</v>
+      </c>
+      <c r="U76" t="str">
+        <f t="shared" si="13"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="V76">
+        <v>0</v>
+      </c>
+      <c r="W76" t="str">
+        <f t="shared" si="14"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>1</v>
       </c>
@@ -4777,32 +6917,60 @@
         <v>0</v>
       </c>
       <c r="I77" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="J77">
         <v>0</v>
       </c>
       <c r="K77" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="L77">
         <v>0</v>
       </c>
       <c r="M77" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="N77">
         <v>0</v>
       </c>
       <c r="O77" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0</v>
       </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P77">
+        <v>0</v>
+      </c>
+      <c r="Q77" t="str">
+        <f t="shared" si="15"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="R77">
+        <v>0</v>
+      </c>
+      <c r="S77" t="str">
+        <f t="shared" si="12"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="T77">
+        <v>0</v>
+      </c>
+      <c r="U77" t="str">
+        <f t="shared" si="13"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="V77">
+        <v>0</v>
+      </c>
+      <c r="W77" t="str">
+        <f t="shared" si="14"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>2</v>
       </c>
@@ -4828,32 +6996,60 @@
         <v>0</v>
       </c>
       <c r="I78" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="J78">
         <v>0</v>
       </c>
       <c r="K78" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="L78">
         <v>0</v>
       </c>
       <c r="M78" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="N78">
         <v>0</v>
       </c>
       <c r="O78" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0 0</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P78">
+        <v>0</v>
+      </c>
+      <c r="Q78" t="str">
+        <f t="shared" si="15"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="R78">
+        <v>0</v>
+      </c>
+      <c r="S78" t="str">
+        <f t="shared" si="12"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="T78">
+        <v>0</v>
+      </c>
+      <c r="U78" t="str">
+        <f t="shared" si="13"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="V78">
+        <v>0</v>
+      </c>
+      <c r="W78" t="str">
+        <f t="shared" si="14"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>2</v>
       </c>
@@ -4879,32 +7075,60 @@
         <v>0</v>
       </c>
       <c r="I79" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="J79">
         <v>0</v>
       </c>
       <c r="K79" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="L79">
         <v>0</v>
       </c>
       <c r="M79" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="N79">
         <v>0</v>
       </c>
       <c r="O79" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0 0 0</v>
       </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P79">
+        <v>0</v>
+      </c>
+      <c r="Q79" t="str">
+        <f t="shared" si="15"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="R79">
+        <v>0</v>
+      </c>
+      <c r="S79" t="str">
+        <f t="shared" si="12"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="T79">
+        <v>0</v>
+      </c>
+      <c r="U79" t="str">
+        <f t="shared" si="13"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="V79">
+        <v>0</v>
+      </c>
+      <c r="W79" t="str">
+        <f t="shared" si="14"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 0 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>2</v>
       </c>
@@ -4930,32 +7154,60 @@
         <v>0</v>
       </c>
       <c r="I80" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="J80">
         <v>0</v>
       </c>
       <c r="K80" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="L80">
         <v>0</v>
       </c>
       <c r="M80" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="N80">
         <v>0</v>
       </c>
       <c r="O80" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0 0 0 0</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P80">
+        <v>0</v>
+      </c>
+      <c r="Q80" t="str">
+        <f t="shared" si="15"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="R80">
+        <v>0</v>
+      </c>
+      <c r="S80" t="str">
+        <f t="shared" si="12"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="T80">
+        <v>0</v>
+      </c>
+      <c r="U80" t="str">
+        <f t="shared" si="13"/>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="V80">
+        <v>0</v>
+      </c>
+      <c r="W80" t="str">
+        <f t="shared" si="14"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 0 0 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>2</v>
       </c>
@@ -4981,32 +7233,61 @@
         <v>0</v>
       </c>
       <c r="I81" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>-0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="J81">
         <v>0</v>
       </c>
       <c r="K81" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="L81">
         <v>0</v>
       </c>
       <c r="M81" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0 0 0 0 0 0</v>
       </c>
       <c r="N81">
         <v>0</v>
       </c>
       <c r="O81" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 -0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0.25 0 0 0 0 0 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="P81">
+        <v>0</v>
+      </c>
+      <c r="Q81" t="str">
+        <f t="shared" si="15"/>
+        <v>0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0.0625 -0.0625 0.0625 -0.0625 0 0 0 0 0 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="R81">
+        <v>0</v>
+      </c>
+      <c r="S81" t="str">
+        <f t="shared" si="12"/>
+        <v>-0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 -0.0625 0.0625 -0.0625 0.0625 0 0 0 0 0 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="T81">
+        <v>0</v>
+      </c>
+      <c r="U81" t="str">
+        <f>U80&amp;" "&amp;T81</f>
+        <v>0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0.125 -0.125 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0</v>
+      </c>
+      <c r="V81">
+        <v>0</v>
+      </c>
+      <c r="W81" t="str">
+        <f t="shared" si="14"/>
+        <v>-0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 -0.125 0.125 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>